<commit_message>
More work on ACWeightsManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/CS300/WEIGHTS/Weights.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -37,12 +37,6 @@
     <t>nmi</t>
   </si>
   <si>
-    <t>Material density</t>
-  </si>
-  <si>
-    <t>kg/m³</t>
-  </si>
-  <si>
     <t>Single passenger Mass</t>
   </si>
   <si>
@@ -61,91 +55,43 @@
     <t>Maximum Landing Mass</t>
   </si>
   <si>
+    <t>Maximum Fuel Mass</t>
+  </si>
+  <si>
+    <t>Design Mission Fuel Mass</t>
+  </si>
+  <si>
+    <t>Maximum Zero Fuel Mass</t>
+  </si>
+  <si>
+    <t>Zero Fuel Mass</t>
+  </si>
+  <si>
     <t>Maximum Passengers Mass</t>
   </si>
   <si>
     <t>Actual Passengers Mass</t>
   </si>
   <si>
-    <t>Maximum Fuel Mass</t>
-  </si>
-  <si>
-    <t>Fuel Mass</t>
+    <t>Operating Empty Mass</t>
+  </si>
+  <si>
+    <t>Empty Mass</t>
+  </si>
+  <si>
+    <t>Trapped Fuel Oil Mass</t>
   </si>
   <si>
     <t>Crew Mass</t>
   </si>
   <si>
-    <t>Maximum Zero Fuel Mass</t>
-  </si>
-  <si>
-    <t>Zero Fuel Mass</t>
-  </si>
-  <si>
-    <t>Operating Empty Mass</t>
-  </si>
-  <si>
-    <t>Empty Mass</t>
+    <t>Operating Item Mass</t>
   </si>
   <si>
     <t>Manufacturer Empty Mass</t>
   </si>
   <si>
-    <t>Operating Item Mass</t>
-  </si>
-  <si>
-    <t>Furnishings and Equipments Mass</t>
-  </si>
-  <si>
-    <t>Trapped Fuel Oil Mass</t>
-  </si>
-  <si>
-    <t>Maximum Take-Off Weight</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Take-Off Weight</t>
-  </si>
-  <si>
-    <t>Maximum Landing Weight</t>
-  </si>
-  <si>
-    <t>Maximum Passengers Weight</t>
-  </si>
-  <si>
-    <t>Actual Passengers Weight</t>
-  </si>
-  <si>
-    <t>Fuel Weight</t>
-  </si>
-  <si>
-    <t>Crew Weight</t>
-  </si>
-  <si>
-    <t>Maximum Zero Fuel Weight</t>
-  </si>
-  <si>
-    <t>Zero Fuel Weight</t>
-  </si>
-  <si>
-    <t>Operating Empty Weight</t>
-  </si>
-  <si>
-    <t>Empty Weight</t>
-  </si>
-  <si>
-    <t>Manufacturer Empty Weight</t>
-  </si>
-  <si>
-    <t>Operating Item Weight</t>
-  </si>
-  <si>
-    <t>Furnishings and Equipments Weight</t>
-  </si>
-  <si>
-    <t>Trapped Fuel Oil Weight</t>
+    <t>Structural Mass</t>
   </si>
   <si>
     <t>Percent Error</t>
@@ -154,7 +100,16 @@
     <t>Reference Mass</t>
   </si>
   <si>
-    <t>Mass Correction Factor</t>
+    <t xml:space="preserve">Estimated Mass </t>
+  </si>
+  <si>
+    <t>Calibration Factor</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Estimated Mass (calibrated)</t>
   </si>
   <si>
     <t>WEIGHT ESTIMATION METHODS COMPARISON</t>
@@ -163,7 +118,13 @@
     <t>JENKINSON</t>
   </si>
   <si>
-    <t>Kg</t>
+    <t>ROSKAM</t>
+  </si>
+  <si>
+    <t>KROO</t>
+  </si>
+  <si>
+    <t>TORENBEEK_2013</t>
   </si>
   <si>
     <t>NICOLAI_1984</t>
@@ -172,31 +133,28 @@
     <t>RAYMER</t>
   </si>
   <si>
-    <t>ROSKAM</t>
-  </si>
-  <si>
-    <t>SADRAY</t>
-  </si>
-  <si>
-    <t>TORENBEEK_2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated Mass </t>
-  </si>
-  <si>
-    <t>Composite Correction Factor</t>
-  </si>
-  <si>
-    <t>KROO</t>
+    <t>TORENBEEK_1976</t>
+  </si>
+  <si>
+    <t>SADRAEY</t>
   </si>
   <si>
     <t>TORENBEEK_1982</t>
   </si>
   <si>
+    <t>NICOLAI_2013</t>
+  </si>
+  <si>
+    <t>HOWE</t>
+  </si>
+  <si>
     <t>Total Reference Mass</t>
   </si>
   <si>
-    <t>Total mass estimated</t>
+    <t>Total Mass Estimated</t>
+  </si>
+  <si>
+    <t>Total Mass Estimated (calibrated)</t>
   </si>
   <si>
     <t>WEIGHT ESTIMATION METHODS COMPARISON FOR EACH NACELLE</t>
@@ -205,31 +163,73 @@
     <t>NACELLE 1</t>
   </si>
   <si>
-    <t>TORENBEEK_1976</t>
+    <t>KUNDU</t>
   </si>
   <si>
     <t>NACELLE 2</t>
   </si>
   <si>
-    <t>Total Dry Mass</t>
-  </si>
-  <si>
     <t>WEIGHT ESTIMATION METHODS COMPARISON FOR EACH ENGINE</t>
   </si>
   <si>
     <t>ENGINE 1</t>
   </si>
   <si>
-    <t>Dry Mass</t>
-  </si>
-  <si>
-    <t>Total Mass</t>
-  </si>
-  <si>
     <t>ENGINE 2</t>
   </si>
   <si>
-    <t>STANFORD</t>
+    <t>Overall Reference Mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Overall Mass </t>
+  </si>
+  <si>
+    <t>Estimated Overall Mass (calibrated)</t>
+  </si>
+  <si>
+    <t>OVERALL WEIGHT:</t>
+  </si>
+  <si>
+    <t>FRONT GEAR WEIGHT:</t>
+  </si>
+  <si>
+    <t>MAIN GEAR WEIGHT:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall Estimated Mass </t>
+  </si>
+  <si>
+    <t>Overall Estimated Mass (calibrated)</t>
+  </si>
+  <si>
+    <t>Method: ALL</t>
+  </si>
+  <si>
+    <t>APU:</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Mass (calibrated)</t>
+  </si>
+  <si>
+    <t>AIR CONDITIONING AND ANTI-ICING SYSTEM:</t>
+  </si>
+  <si>
+    <t>INSTRUMENTS AND NAVIGATION SYSTEM:</t>
+  </si>
+  <si>
+    <t>HYDRAULIC AND PNEUMATIC SYSTEMS:</t>
+  </si>
+  <si>
+    <t>ELECTRICAL SYSTEMS:</t>
+  </si>
+  <si>
+    <t>CONTROL SURFACES:</t>
+  </si>
+  <si>
+    <t>FURNISHINGS AND EQUIPMENTS:</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>3200.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="3">
@@ -331,369 +331,188 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>2711.0</v>
+        <v>106.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>105.0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>231674.74431825435</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>55106.72117531574</v>
+        <v>229554.74431825435</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>54686.72117531574</v>
+        <v>224724.5019887067</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>53453.519540056266</v>
+        <v>13149.651482339104</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>7560.0</v>
+        <v>64481.45269232038</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>7140.0</v>
+        <v>167193.291625934</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>14372.170291875165</v>
+        <v>165073.291625934</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>15478.475137969412</v>
+        <v>15900.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>229.54364550000003</v>
+        <v>13780.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>39628.24603734633</v>
+        <v>151293.291625934</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>39208.24603734633</v>
+        <v>149752.4176231049</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>32068.246037346336</v>
+        <v>1158.3012603290836</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>31563.168785940274</v>
+        <v>382.5727425</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>30760.862391846338</v>
+        <v>2245.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>1077.8400000000001</v>
+        <v>148665.21888343405</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>2564.6197223312765</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="n">
-        <v>275.5336059060588</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" t="n">
-        <v>540412.32721391</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" t="n">
-        <v>536293.5342139099</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="n">
-        <v>524199.9573974926</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="n">
-        <v>74138.27399999998</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="n">
-        <v>70019.48099999997</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="n">
-        <v>140942.84379281756</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" t="n">
-        <v>2251.0541911425744</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" t="n">
-        <v>388620.3390021423</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" t="n">
-        <v>384501.54600214225</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="n">
-        <v>314482.06500214234</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="n">
-        <v>309528.94917464105</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" t="n">
-        <v>301661.0111749998</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" t="n">
-        <v>10569.999635999997</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="n">
-        <v>25150.328000000005</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C37" t="n">
-        <v>2702.0616363586505</v>
+        <v>126432.39304354903</v>
       </c>
     </row>
   </sheetData>
@@ -724,137 +543,176 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>7603.312499999998</v>
+        <v>23166.025206581675</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>10800.375</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-53.37838535662337</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10800.374999999998</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="n">
-        <v>9258.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>21.76271855194696</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6390.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-15.957682917807187</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>6016.0</v>
+        <v>9233.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-20.876591617140537</v>
+        <v>-60.14422017732752</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>6546.0</v>
+        <v>26315.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-13.905945599368676</v>
+        <v>13.593073327588685</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>6396.0</v>
+        <v>7573.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-15.87876994402109</v>
+        <v>-67.30988621281288</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
         <v>7891.0</v>
       </c>
       <c r="D11" t="n">
-        <v>3.783712691014632</v>
+        <v>-65.93718633372593</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>7082.833333333332</v>
+        <v>10219.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-6.845426472562652</v>
+        <v>-55.887987218900676</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12315.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-46.8402546825288</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6461.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-72.11001912333079</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6396.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-72.39060243194919</v>
       </c>
     </row>
   </sheetData>
@@ -885,37 +743,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>5068.874999999998</v>
+        <v>24555.98671897657</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>11886.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-51.59632501831153</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -923,124 +784,121 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11885.999999999998</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-100.0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>6335.0</v>
+        <v>14322.0</v>
       </c>
       <c r="D8" t="n">
-        <v>24.97842223373041</v>
+        <v>-41.67613721287716</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>6115.0</v>
+        <v>12068.0</v>
       </c>
       <c r="D9" t="n">
-        <v>20.638208675495097</v>
+        <v>-50.855161561583685</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>7434.0</v>
+        <v>1327.0</v>
       </c>
       <c r="D10" t="n">
-        <v>46.65976178146043</v>
+        <v>-94.59602248858315</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>5911.0</v>
+        <v>18805.0</v>
       </c>
       <c r="D11" t="n">
-        <v>16.613647012404172</v>
+        <v>-23.419896682597052</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>7919.0</v>
+        <v>14233.0</v>
       </c>
       <c r="D12" t="n">
-        <v>56.22795985302464</v>
+        <v>-42.03857428787045</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>6736.0</v>
+        <v>16646.0</v>
       </c>
       <c r="D13" t="n">
-        <v>32.889447855786585</v>
+        <v>-32.21204999619838</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>5778.5714285714275</v>
+        <v>5801.0</v>
       </c>
       <c r="D14" t="n">
-        <v>14.001063915985885</v>
+        <v>-76.37643289847091</v>
       </c>
     </row>
   </sheetData>
@@ -1071,37 +929,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>760.3312499999997</v>
+        <v>2664.0928987568923</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>808.2857142857142</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-69.6600026724716</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -1109,68 +970,121 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>808.2857142857142</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="n">
-        <v>642.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-15.563118048876692</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>269.0</v>
+        <v>1022.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-64.62068341923337</v>
+        <v>-61.63797439357759</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>472.0</v>
+        <v>700.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-37.92179395493738</v>
+        <v>-73.7246399956011</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>461.0</v>
+        <v>482.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-39.36853180768248</v>
+        <v>-81.90753782554246</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>783.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-70.60913302365093</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>472.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-82.28290011131959</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1138.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-57.283771878562916</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1061.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-60.17406147904679</v>
       </c>
     </row>
   </sheetData>
@@ -1201,37 +1115,40 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>760.3312499999997</v>
+        <v>2664.0928987568923</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>568.1666666666665</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-78.67316612976288</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -1239,54 +1156,107 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>568.1666666666665</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" t="n">
-        <v>502.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-33.97614526563255</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>441.0</v>
+        <v>502.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-41.99896426721904</v>
+        <v>-81.1568132539882</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>471.5</v>
+        <v>482.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-37.98755476642579</v>
+        <v>-81.90753782554246</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>933.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-64.97869873699402</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>382.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-85.66116068331374</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>363.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-86.37434902629028</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>747.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-71.96043725244859</v>
       </c>
     </row>
   </sheetData>
@@ -1317,191 +1287,213 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>760.3312499999997</v>
+        <v>4401.544789250517</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1108.6666666666665</v>
+        <v>97373.33333333331</v>
       </c>
       <c r="D3" t="n">
-        <v>-51.39545355323014</v>
+        <v>2112.2536063052034</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>97373.3333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" t="n">
-        <v>705.0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>85.4454883973269</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>377.0</v>
+        <v>1410.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.8326962754720038</v>
+        <v>12.447192334220247</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>581.0</v>
+        <v>3029.0</v>
       </c>
       <c r="D11" t="n">
-        <v>52.828125899073655</v>
+        <v>141.56208906408023</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>554.3333333333333</v>
+        <v>141621.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>11194.24384791816</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>48686.66666666666</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="n">
-        <v>705.0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>85.4454883973269</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>377.0</v>
+        <v>1410.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.8326962754720038</v>
+        <v>12.447192334220247</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>581.0</v>
+        <v>3029.0</v>
       </c>
       <c r="D18" t="n">
-        <v>52.828125899073655</v>
+        <v>141.56208906408023</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>554.3333333333333</v>
+        <v>141621.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>11194.24384791816</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>48686.66666666666</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1531,106 +1523,214 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>4353.999999999998</v>
+        <v>19227.80092146279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>6915.896865902219</v>
+        <v>6451.333333333332</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-66.44788782823255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6451.333333333331</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2177.0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3457.9484329511106</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3458.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-17.267576363460925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>2177.0</v>
+        <v>2954.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-29.32574337121561</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>3457.9484329511106</v>
+        <v>3265.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-21.885088729525716</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3225.666666666666</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3458.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-17.267576363460925</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2954.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-29.32574337121561</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3265.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-21.885088729525716</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3225.666666666666</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1661,98 +1761,115 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2027.5499999999995</v>
+        <v>9498.070334698485</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4996.232329263368</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-47.3973959635668</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>1591.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-21.530911691450246</v>
+        <v>4996.232329263368</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2204.0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8.702621390347996</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2514.0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>23.9920100614042</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2233.0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>10.132919040220996</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>2135.5</v>
+        <v>4996.232329263369</v>
       </c>
       <c r="D9" t="n">
-        <v>5.324159700130713</v>
+        <v>-47.39739596356681</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.59451512125535</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4990.637814142114</v>
       </c>
     </row>
   </sheetData>
@@ -1783,56 +1900,373 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2027.5499999999995</v>
+        <v>31505.79428095107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15781.492506551778</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-49.90923775537525</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15781.492506551778</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="n">
-        <v>4242.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>109.21802175038847</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4242.2743750414265</v>
-      </c>
-      <c r="D6" t="n">
-        <v>109.23155409442067</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15781.49250655178</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-49.909237755375266</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>322.1932175083158</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>322.19321750831574</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
+        <v>706.4578234830049</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>706.4578234830047</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2292.6345773225576</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2292.634577322557</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2229.9227611289743</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2229.922761128974</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1542.6061340651304</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1542.6061340651302</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1854.6844619981066</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1854.6844619981064</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="n">
+        <v>6832.993531045695</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="n">
+        <v>6832.993531045694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on ACWeightsManager and JPADResponseSurfaceOptimizer.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/WEIGHTS/Weights.xlsx
+++ b/JPADSandBox_v2/out/CS300/WEIGHTS/Weights.xlsx
@@ -347,7 +347,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>231674.74431825435</v>
+        <v>67704.39484783061</v>
       </c>
     </row>
     <row r="6">
@@ -358,7 +358,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>229554.74431825435</v>
+        <v>67704.39484783061</v>
       </c>
     </row>
     <row r="7">
@@ -369,7 +369,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>224724.5019887067</v>
+        <v>65673.26300239567</v>
       </c>
     </row>
     <row r="8">
@@ -391,7 +391,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>64481.45269232038</v>
+        <v>18846.614647889844</v>
       </c>
     </row>
     <row r="10">
@@ -402,7 +402,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>167193.291625934</v>
+        <v>48857.78019994077</v>
       </c>
     </row>
     <row r="11">
@@ -413,7 +413,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>165073.291625934</v>
+        <v>48857.78019994077</v>
       </c>
     </row>
     <row r="12">
@@ -424,7 +424,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>15900.0</v>
+        <v>13780.0</v>
       </c>
     </row>
     <row r="13">
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>151293.291625934</v>
+        <v>35077.780199940775</v>
       </c>
     </row>
     <row r="15">
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>149752.4176231049</v>
+        <v>34356.65960238931</v>
       </c>
     </row>
     <row r="16">
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>1158.3012603290836</v>
+        <v>338.54785505146185</v>
       </c>
     </row>
     <row r="17">
@@ -490,7 +490,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>2245.5</v>
+        <v>1946.1</v>
       </c>
     </row>
     <row r="19">
@@ -501,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>148665.21888343405</v>
+        <v>32749.10745744078</v>
       </c>
     </row>
     <row r="20">
@@ -512,7 +512,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>126432.39304354903</v>
+        <v>18334.760616664655</v>
       </c>
     </row>
   </sheetData>
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>23166.025206581675</v>
+        <v>6770.957101029237</v>
       </c>
     </row>
     <row r="3">
@@ -565,10 +565,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>10800.375</v>
+        <v>7282.5</v>
       </c>
       <c r="D3" t="n">
-        <v>-53.37838535662337</v>
+        <v>7.554957022146899</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>10800.374999999998</v>
+        <v>7282.499999999999</v>
       </c>
     </row>
     <row r="6">
@@ -614,7 +614,7 @@
         <v>9233.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-60.14422017732752</v>
+        <v>36.361815061514925</v>
       </c>
     </row>
     <row r="9">
@@ -625,10 +625,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>26315.0</v>
+        <v>8179.0</v>
       </c>
       <c r="D9" t="n">
-        <v>13.593073327588685</v>
+        <v>20.79533037887259</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>7573.0</v>
+        <v>6502.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-67.30988621281288</v>
+        <v>-3.972216881840133</v>
       </c>
     </row>
     <row r="11">
@@ -656,7 +656,7 @@
         <v>7891.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-65.93718633372593</v>
+        <v>16.541869668624965</v>
       </c>
     </row>
     <row r="12">
@@ -667,10 +667,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>10219.0</v>
+        <v>6940.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-55.887987218900676</v>
+        <v>2.4965879483281266</v>
       </c>
     </row>
     <row r="13">
@@ -681,10 +681,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>12315.0</v>
+        <v>6658.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-46.8402546825288</v>
+        <v>-1.6682589971226705</v>
       </c>
     </row>
     <row r="14">
@@ -698,7 +698,7 @@
         <v>6461.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-72.11001912333079</v>
+        <v>-4.57774427461844</v>
       </c>
     </row>
     <row r="15">
@@ -712,7 +712,7 @@
         <v>6396.0</v>
       </c>
       <c r="D15" t="n">
-        <v>-72.39060243194919</v>
+        <v>-5.537726726584049</v>
       </c>
     </row>
   </sheetData>
@@ -754,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>24555.98671897657</v>
+        <v>7177.2145270909905</v>
       </c>
     </row>
     <row r="3">
@@ -765,10 +765,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>11886.0</v>
+        <v>5492.428571428571</v>
       </c>
       <c r="D3" t="n">
-        <v>-51.59632501831153</v>
+        <v>-23.474092202525853</v>
       </c>
     </row>
     <row r="4">
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>11885.999999999998</v>
+        <v>5492.428571428571</v>
       </c>
     </row>
     <row r="6">
@@ -811,10 +811,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>14322.0</v>
+        <v>6054.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-41.67613721287716</v>
+        <v>-15.64972766038027</v>
       </c>
     </row>
     <row r="9">
@@ -825,10 +825,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>12068.0</v>
+        <v>4294.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-50.855161561583685</v>
+        <v>-40.1717757802565</v>
       </c>
     </row>
     <row r="10">
@@ -839,10 +839,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>1327.0</v>
+        <v>894.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-94.59602248858315</v>
+        <v>-87.54391419365378</v>
       </c>
     </row>
     <row r="11">
@@ -853,10 +853,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>18805.0</v>
+        <v>7143.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-23.419896682597052</v>
+        <v>-0.4767103862068497</v>
       </c>
     </row>
     <row r="12">
@@ -867,10 +867,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>14233.0</v>
+        <v>5871.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-42.03857428787045</v>
+        <v>-18.199463345571946</v>
       </c>
     </row>
     <row r="13">
@@ -881,10 +881,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>16646.0</v>
+        <v>8390.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-32.21204999619838</v>
+        <v>16.897718026000913</v>
       </c>
     </row>
     <row r="14">
@@ -898,7 +898,7 @@
         <v>5801.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-76.37643289847091</v>
+        <v>-19.174772077612477</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +940,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2664.0928987568923</v>
+        <v>778.6600666183622</v>
       </c>
     </row>
     <row r="3">
@@ -951,10 +951,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>808.2857142857142</v>
+        <v>625.7142857142856</v>
       </c>
       <c r="D3" t="n">
-        <v>-69.6600026724716</v>
+        <v>-19.642176022754548</v>
       </c>
     </row>
     <row r="4">
@@ -976,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>808.2857142857142</v>
+        <v>625.7142857142856</v>
       </c>
     </row>
     <row r="6">
@@ -997,10 +997,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>1022.0</v>
+        <v>409.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-61.63797439357759</v>
+        <v>-47.4738698523165</v>
       </c>
     </row>
     <row r="9">
@@ -1014,7 +1014,7 @@
         <v>700.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-73.7246399956011</v>
+        <v>-10.10197774235097</v>
       </c>
     </row>
     <row r="10">
@@ -1028,7 +1028,7 @@
         <v>482.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-81.90753782554246</v>
+        <v>-38.09879038830452</v>
       </c>
     </row>
     <row r="11">
@@ -1039,10 +1039,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>783.0</v>
+        <v>737.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-70.60913302365093</v>
+        <v>-5.3502251373038066</v>
       </c>
     </row>
     <row r="12">
@@ -1056,7 +1056,7 @@
         <v>472.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-82.28290011131959</v>
+        <v>-39.38304784912808</v>
       </c>
     </row>
     <row r="13">
@@ -1067,10 +1067,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>1138.0</v>
+        <v>519.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-57.283771878562916</v>
+        <v>-33.34703778325736</v>
       </c>
     </row>
     <row r="14">
@@ -1084,7 +1084,7 @@
         <v>1061.0</v>
       </c>
       <c r="D14" t="n">
-        <v>-60.17406147904679</v>
+        <v>36.25971659337946</v>
       </c>
     </row>
   </sheetData>
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2664.0928987568923</v>
+        <v>778.6600666183622</v>
       </c>
     </row>
     <row r="3">
@@ -1137,10 +1137,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>568.1666666666665</v>
+        <v>465.66666666666663</v>
       </c>
       <c r="D3" t="n">
-        <v>-78.67316612976288</v>
+        <v>-40.19641090764966</v>
       </c>
     </row>
     <row r="4">
@@ -1162,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>568.1666666666665</v>
+        <v>465.66666666666663</v>
       </c>
     </row>
     <row r="6">
@@ -1186,7 +1186,7 @@
         <v>502.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-81.1568132539882</v>
+        <v>-35.53027546665741</v>
       </c>
     </row>
     <row r="9">
@@ -1200,7 +1200,7 @@
         <v>482.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-81.90753782554246</v>
+        <v>-38.09879038830452</v>
       </c>
     </row>
     <row r="10">
@@ -1211,10 +1211,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>933.0</v>
+        <v>498.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-64.97869873699402</v>
+        <v>-36.043978450986835</v>
       </c>
     </row>
     <row r="11">
@@ -1228,7 +1228,7 @@
         <v>382.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-85.66116068331374</v>
+        <v>-50.9413649965401</v>
       </c>
     </row>
     <row r="12">
@@ -1239,10 +1239,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>363.0</v>
+        <v>183.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-86.37434902629028</v>
+        <v>-76.49808846692889</v>
       </c>
     </row>
     <row r="13">
@@ -1256,7 +1256,7 @@
         <v>747.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-71.96043725244859</v>
+        <v>-4.065967676480249</v>
       </c>
     </row>
   </sheetData>
@@ -1298,7 +1298,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>4401.544789250517</v>
+        <v>2572.9636983911096</v>
       </c>
     </row>
     <row r="3">
@@ -1309,10 +1309,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>97373.33333333331</v>
+        <v>2782.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2112.2536063052034</v>
+        <v>8.124339326652846</v>
       </c>
     </row>
     <row r="4">
@@ -1334,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>97373.3333333333</v>
+        <v>2781.9999999999995</v>
       </c>
     </row>
     <row r="6">
@@ -1368,7 +1368,7 @@
         <v>1410.0</v>
       </c>
       <c r="D10" t="n">
-        <v>12.447192334220247</v>
+        <v>9.601235406599937</v>
       </c>
     </row>
     <row r="11">
@@ -1379,10 +1379,10 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>3029.0</v>
+        <v>1374.0</v>
       </c>
       <c r="D11" t="n">
-        <v>141.56208906408023</v>
+        <v>6.802905991963343</v>
       </c>
     </row>
     <row r="12">
@@ -1393,10 +1393,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>141621.0</v>
+        <v>1389.0</v>
       </c>
       <c r="D12" t="n">
-        <v>11194.24384791816</v>
+        <v>7.968876581395257</v>
       </c>
     </row>
     <row r="13">
@@ -1416,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>48686.66666666666</v>
+        <v>1391.0</v>
       </c>
     </row>
     <row r="15">
@@ -1440,7 +1440,7 @@
         <v>1410.0</v>
       </c>
       <c r="D17" t="n">
-        <v>12.447192334220247</v>
+        <v>9.601235406599937</v>
       </c>
     </row>
     <row r="18">
@@ -1451,10 +1451,10 @@
         <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>3029.0</v>
+        <v>1374.0</v>
       </c>
       <c r="D18" t="n">
-        <v>141.56208906408023</v>
+        <v>6.802905991963343</v>
       </c>
     </row>
     <row r="19">
@@ -1465,10 +1465,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>141621.0</v>
+        <v>1389.0</v>
       </c>
       <c r="D19" t="n">
-        <v>11194.24384791816</v>
+        <v>7.968876581395257</v>
       </c>
     </row>
     <row r="20">
@@ -1488,7 +1488,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>48686.66666666666</v>
+        <v>1391.0</v>
       </c>
     </row>
     <row r="22">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>19227.80092146279</v>
+        <v>5619.894393854267</v>
       </c>
     </row>
     <row r="3">
@@ -1549,7 +1549,7 @@
         <v>6451.333333333332</v>
       </c>
       <c r="D3" t="n">
-        <v>-66.44788782823255</v>
+        <v>14.794565185927684</v>
       </c>
     </row>
     <row r="4">
@@ -1614,7 +1614,7 @@
         <v>3458.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-17.267576363460925</v>
+        <v>23.062810709808247</v>
       </c>
     </row>
     <row r="12">
@@ -1628,7 +1628,7 @@
         <v>2954.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-29.32574337121561</v>
+        <v>5.126530606354414</v>
       </c>
     </row>
     <row r="13">
@@ -1642,7 +1642,7 @@
         <v>3265.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-21.885088729525716</v>
+        <v>16.19435424162057</v>
       </c>
     </row>
     <row r="14">
@@ -1686,7 +1686,7 @@
         <v>3458.0</v>
       </c>
       <c r="D18" t="n">
-        <v>-17.267576363460925</v>
+        <v>23.062810709808247</v>
       </c>
     </row>
     <row r="19">
@@ -1700,7 +1700,7 @@
         <v>2954.0</v>
       </c>
       <c r="D19" t="n">
-        <v>-29.32574337121561</v>
+        <v>5.126530606354414</v>
       </c>
     </row>
     <row r="20">
@@ -1714,7 +1714,7 @@
         <v>3265.0</v>
       </c>
       <c r="D20" t="n">
-        <v>-21.885088729525716</v>
+        <v>16.19435424162057</v>
       </c>
     </row>
     <row r="21">
@@ -1772,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>9498.070334698485</v>
+        <v>2776.092411421987</v>
       </c>
     </row>
     <row r="3">
@@ -1783,10 +1783,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>4996.232329263368</v>
+        <v>1686.451092855138</v>
       </c>
       <c r="D3" t="n">
-        <v>-47.3973959635668</v>
+        <v>-39.25090224243314</v>
       </c>
     </row>
     <row r="4">
@@ -1808,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>4996.232329263368</v>
+        <v>1686.4510928551379</v>
       </c>
     </row>
     <row r="6">
@@ -1834,10 +1834,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>4996.232329263369</v>
+        <v>1686.451092855138</v>
       </c>
       <c r="D9" t="n">
-        <v>-47.39739596356681</v>
+        <v>-39.25090224243314</v>
       </c>
     </row>
     <row r="10">
@@ -1853,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>5.59451512125535</v>
+        <v>216.94217584712888</v>
       </c>
     </row>
     <row r="12">
@@ -1869,7 +1869,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>4990.637814142114</v>
+        <v>1469.5089170080093</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>31505.79428095107</v>
+        <v>9208.501657399762</v>
       </c>
     </row>
     <row r="3">
@@ -1922,10 +1922,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>15781.492506551778</v>
+        <v>7963.013507442807</v>
       </c>
       <c r="D3" t="n">
-        <v>-49.90923775537525</v>
+        <v>-13.525415928617502</v>
       </c>
     </row>
     <row r="4">
@@ -1936,7 +1936,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>15781.492506551778</v>
+        <v>7963.013507442807</v>
       </c>
     </row>
     <row r="5">
@@ -1962,10 +1962,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>15781.49250655178</v>
+        <v>7963.013507442808</v>
       </c>
       <c r="D8" t="n">
-        <v>-49.909237755375266</v>
+        <v>-13.525415928617482</v>
       </c>
     </row>
     <row r="9">
@@ -2072,7 +2072,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>2292.6345773225576</v>
+        <v>989.3371461547074</v>
       </c>
     </row>
     <row r="22">
@@ -2094,7 +2094,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>2292.634577322557</v>
+        <v>989.3371461547073</v>
       </c>
     </row>
     <row r="24">
@@ -2115,7 +2115,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>2229.9227611289743</v>
+        <v>491.2608278969228</v>
       </c>
     </row>
     <row r="27">
@@ -2137,7 +2137,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>2229.922761128974</v>
+        <v>491.26082789692276</v>
       </c>
     </row>
     <row r="29">
@@ -2201,7 +2201,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="n">
-        <v>1854.6844619981066</v>
+        <v>816.8041180658586</v>
       </c>
     </row>
     <row r="37">
@@ -2223,7 +2223,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="n">
-        <v>1854.6844619981064</v>
+        <v>816.8041180658585</v>
       </c>
     </row>
     <row r="39">
@@ -2244,7 +2244,7 @@
         <v>6</v>
       </c>
       <c r="C41" t="n">
-        <v>6832.993531045695</v>
+        <v>3094.35424026887</v>
       </c>
     </row>
     <row r="42">
@@ -2266,7 +2266,7 @@
         <v>6</v>
       </c>
       <c r="C43" t="n">
-        <v>6832.993531045694</v>
+        <v>3094.35424026887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>